<commit_message>
fixed problem with deleting wrong element in forecast error arrays in simulations
</commit_message>
<xml_diff>
--- a/BrockMirman/BM Table.xlsx
+++ b/BrockMirman/BM Table.xlsx
@@ -9,10 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="11000" windowHeight="15000"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="19380" windowHeight="15000"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table" sheetId="1" r:id="rId1"/>
+    <sheet name="EX" sheetId="4" r:id="rId2"/>
+    <sheet name="LIN" sheetId="3" r:id="rId3"/>
+    <sheet name="GSSA" sheetId="5" r:id="rId4"/>
+    <sheet name="VFI" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="21">
   <si>
     <t>EX</t>
   </si>
@@ -60,6 +64,33 @@
   </si>
   <si>
     <t>Simulate</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -427,7 +458,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -485,6 +516,9 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
+      <c r="C9">
+        <v>2.5195099999999999E-4</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
@@ -494,6 +528,9 @@
     <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
       </c>
       <c r="C11" s="2">
         <v>1.8518824345174754E-3</v>
@@ -514,4 +551,409 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F10"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>5.1924099999999997E-3</v>
+      </c>
+      <c r="D3">
+        <v>0.16939299999999999</v>
+      </c>
+      <c r="E3">
+        <v>1.2332600000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>9.1803099999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>6.2318800000000004E-3</v>
+      </c>
+      <c r="D4">
+        <v>0.106471</v>
+      </c>
+      <c r="E4">
+        <v>7.2574700000000002E-3</v>
+      </c>
+      <c r="F4">
+        <v>9.09569E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>5.21837E-3</v>
+      </c>
+      <c r="D5">
+        <v>0.123986</v>
+      </c>
+      <c r="E5">
+        <v>3.9627400000000002E-3</v>
+      </c>
+      <c r="F5">
+        <v>4.9671400000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>1.42776E-4</v>
+      </c>
+      <c r="D6">
+        <v>1.1889E-2</v>
+      </c>
+      <c r="E6">
+        <v>3.9897999999999999E-3</v>
+      </c>
+      <c r="F6">
+        <v>5.0004400000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>5.71917E-3</v>
+      </c>
+      <c r="D7">
+        <v>0.45614700000000002</v>
+      </c>
+      <c r="E7">
+        <v>4.3182100000000003E-3</v>
+      </c>
+      <c r="F7">
+        <v>5.4154700000000004E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>5.21909E-3</v>
+      </c>
+      <c r="D8">
+        <v>0.12366199999999999</v>
+      </c>
+      <c r="E8">
+        <v>3.9629799999999996E-3</v>
+      </c>
+      <c r="F8">
+        <v>4.96832E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>4.5296099999999999E-3</v>
+      </c>
+      <c r="D9">
+        <v>0.14741199999999999</v>
+      </c>
+      <c r="E9">
+        <v>1.2892299999999999E-3</v>
+      </c>
+      <c r="F9">
+        <v>1.6389200000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>4.8891100000000003E-3</v>
+      </c>
+      <c r="D10">
+        <v>6.7438100000000001E-2</v>
+      </c>
+      <c r="E10">
+        <v>1.39145E-3</v>
+      </c>
+      <c r="F10">
+        <v>1.7685999999999999E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating results for BM, EX and LIN
</commit_message>
<xml_diff>
--- a/BrockMirman/BM Table.xlsx
+++ b/BrockMirman/BM Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="19380" windowHeight="15000"/>
+    <workbookView xWindow="14160" yWindow="460" windowWidth="10180" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,16 +141,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -458,7 +472,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -486,53 +500,102 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="2">
+        <f>EX!B3</f>
+        <v>2.8961199999999999E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <f>LIN!C3</f>
+        <v>2.8961199999999999E-2</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="2">
+        <f>EX!C3</f>
+        <v>0.40005400000000002</v>
+      </c>
+      <c r="C4" s="2">
+        <f>LIN!D3</f>
+        <v>0.40005400000000002</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="2">
+        <f>EX!D3</f>
+        <v>6.8301600000000004E-2</v>
+      </c>
+      <c r="C6" s="2">
+        <f>LIN!E3</f>
+        <v>6.8301600000000004E-2</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="2">
+        <f>EX!E3</f>
+        <v>0.50732600000000005</v>
+      </c>
+      <c r="C7" s="2">
+        <f>LIN!F3</f>
+        <v>0.50732600000000005</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" s="5" customFormat="1">
+      <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
-        <v>2.5195099999999999E-4</v>
+      <c r="B9" s="5">
+        <v>2.4255199999999999E-4</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2.5194099999999999E-4</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>1.8518824345174754E-3</v>
       </c>
     </row>
@@ -540,10 +603,10 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>31.537829729678734</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>62.380262520635483</v>
       </c>
     </row>
@@ -558,7 +621,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E10"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -589,40 +652,136 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
+      <c r="B3" s="2">
+        <v>2.8961199999999999E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.40005400000000002</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6.8301600000000004E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.50732600000000005</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="2">
+        <v>9.5810300000000008E-3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.132017</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7.25576E-3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9.09482E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>14</v>
       </c>
+      <c r="B5" s="2">
+        <v>1.55158E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.21379300000000001</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.1750200000000001E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.47285E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
+      <c r="B6" s="2">
+        <v>1.4076400000000001E-4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.18049E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.9488500000000003E-3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4.9497400000000002E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>16</v>
       </c>
+      <c r="B7" s="2">
+        <v>0.19162100000000001</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.6403400000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.14511499999999999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.181896</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>17</v>
       </c>
+      <c r="B8" s="2">
+        <v>1.5435000000000001E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.21266299999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.1685600000000001E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.46477E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>18</v>
       </c>
+      <c r="B9" s="2">
+        <v>2.52643E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.34814299999999998</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7.17294E-3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>9.1145700000000007E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>19</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4.5260500000000002E-3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6.4885899999999996E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.2863600000000001E-3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.6358500000000001E-3</v>
       </c>
     </row>
   </sheetData>
@@ -635,7 +794,7 @@
   <dimension ref="B1:F10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F10"/>
+      <selection activeCell="C3" sqref="C3:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -666,136 +825,136 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
-        <v>5.1924099999999997E-3</v>
-      </c>
-      <c r="D3">
-        <v>0.16939299999999999</v>
-      </c>
-      <c r="E3">
-        <v>1.2332600000000001E-2</v>
-      </c>
-      <c r="F3">
-        <v>9.1803099999999999E-2</v>
+      <c r="C3" s="2">
+        <v>2.8961199999999999E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.40005400000000002</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6.8301600000000004E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.50732600000000005</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
-        <v>6.2318800000000004E-3</v>
-      </c>
-      <c r="D4">
-        <v>0.106471</v>
-      </c>
-      <c r="E4">
-        <v>7.2574700000000002E-3</v>
-      </c>
-      <c r="F4">
-        <v>9.09569E-3</v>
+      <c r="C4" s="2">
+        <v>9.5810300000000008E-3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.132017</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7.25576E-3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>9.09482E-3</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5">
-        <v>5.21837E-3</v>
-      </c>
-      <c r="D5">
-        <v>0.123986</v>
-      </c>
-      <c r="E5">
-        <v>3.9627400000000002E-3</v>
-      </c>
-      <c r="F5">
-        <v>4.9671400000000001E-3</v>
+      <c r="C5" s="2">
+        <v>1.55158E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.21379300000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.1750200000000001E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.47285E-2</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
-        <v>1.42776E-4</v>
-      </c>
-      <c r="D6">
-        <v>1.1889E-2</v>
-      </c>
-      <c r="E6">
-        <v>3.9897999999999999E-3</v>
-      </c>
-      <c r="F6">
-        <v>5.0004400000000001E-3</v>
+      <c r="C6" s="2">
+        <v>1.4076400000000001E-4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.18049E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3.9488500000000003E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4.9497400000000002E-3</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
-        <v>5.71917E-3</v>
-      </c>
-      <c r="D7">
-        <v>0.45614700000000002</v>
-      </c>
-      <c r="E7">
-        <v>4.3182100000000003E-3</v>
-      </c>
-      <c r="F7">
-        <v>5.4154700000000004E-3</v>
+      <c r="C7" s="2">
+        <v>0.19162100000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.6403400000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.14511499999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.181896</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8">
-        <v>5.21909E-3</v>
-      </c>
-      <c r="D8">
-        <v>0.12366199999999999</v>
-      </c>
-      <c r="E8">
-        <v>3.9629799999999996E-3</v>
-      </c>
-      <c r="F8">
-        <v>4.96832E-3</v>
+      <c r="C8" s="2">
+        <v>1.5435000000000001E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.21266299999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.1685600000000001E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.46477E-2</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9">
-        <v>4.5296099999999999E-3</v>
-      </c>
-      <c r="D9">
-        <v>0.14741199999999999</v>
-      </c>
-      <c r="E9">
-        <v>1.2892299999999999E-3</v>
-      </c>
-      <c r="F9">
-        <v>1.6389200000000001E-3</v>
+      <c r="C9" s="2">
+        <v>2.52643E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.34814299999999998</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7.17294E-3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>9.1145700000000007E-3</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
-        <v>4.8891100000000003E-3</v>
-      </c>
-      <c r="D10">
-        <v>6.7438100000000001E-2</v>
-      </c>
-      <c r="E10">
-        <v>1.39145E-3</v>
-      </c>
-      <c r="F10">
-        <v>1.7685999999999999E-3</v>
+      <c r="C10" s="2">
+        <v>4.5260500000000002E-3</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6.4885899999999996E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.2863600000000001E-3</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.6358500000000001E-3</v>
       </c>
     </row>
   </sheetData>
@@ -809,7 +968,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E10"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
tweaks to code for RMS Euler Errors; results for BMsimGSSA
</commit_message>
<xml_diff>
--- a/BrockMirman/BM Table.xlsx
+++ b/BrockMirman/BM Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14160" yWindow="460" windowWidth="10180" windowHeight="15000"/>
+    <workbookView xWindow="13880" yWindow="600" windowWidth="10180" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -149,8 +149,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -508,7 +508,10 @@
         <f>LIN!C3</f>
         <v>2.8961199999999999E-2</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <f>GSSA!B3</f>
+        <v>2.90809E-2</v>
+      </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
@@ -523,7 +526,10 @@
         <f>LIN!D3</f>
         <v>0.40005400000000002</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <f>GSSA!C3</f>
+        <v>0.40088000000000001</v>
+      </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
@@ -547,7 +553,10 @@
         <f>LIN!E3</f>
         <v>6.8301600000000004E-2</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <f>GSSA!D3</f>
+        <v>6.8293099999999995E-2</v>
+      </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5">
@@ -562,7 +571,10 @@
         <f>LIN!F3</f>
         <v>0.50732600000000005</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <f>GSSA!E3</f>
+        <v>0.50732500000000003</v>
+      </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5">
@@ -580,6 +592,9 @@
       <c r="C9" s="5">
         <v>2.5194099999999999E-4</v>
       </c>
+      <c r="D9" s="5">
+        <v>2.41043E-4</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
@@ -598,6 +613,9 @@
       <c r="C11" s="3">
         <v>1.8518824345174754E-3</v>
       </c>
+      <c r="D11">
+        <v>173.34756409923267</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
@@ -608,6 +626,9 @@
       </c>
       <c r="C12" s="3">
         <v>62.380262520635483</v>
+      </c>
+      <c r="D12">
+        <v>122.76904415020975</v>
       </c>
     </row>
   </sheetData>
@@ -968,7 +989,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -999,40 +1020,136 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
+      <c r="B3" s="2">
+        <v>2.90809E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.40088000000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6.8293099999999995E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.50732500000000003</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="2">
+        <v>9.6187600000000005E-3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.13227700000000001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7.2549299999999997E-3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9.0941400000000006E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>14</v>
       </c>
+      <c r="B5" s="2">
+        <v>1.5576899999999999E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.21421299999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.17489E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.47274E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
+      <c r="B6" s="2">
+        <v>1.12862E-4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.0570400000000001E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.9484000000000003E-3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4.9493699999999998E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>16</v>
       </c>
+      <c r="B7" s="2">
+        <v>0.19237499999999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.6455299999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.14509900000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.18188299999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>17</v>
       </c>
+      <c r="B8" s="2">
+        <v>1.54935E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.21306600000000001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.1686E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.46485E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>18</v>
       </c>
+      <c r="B9" s="2">
+        <v>2.9220800000000002E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.40184300000000001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8.2620599999999999E-3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.0497100000000001E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>19</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4.5435800000000002E-3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6.5011399999999997E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.2863600000000001E-3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.6361699999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All finished with BM!!  Moved gssa.py inside BMsolveGSSA.py.  Renamed VFI to VFI_11.  Deleted results for VFI with 21 and 31 grid points as they are not needed.  We do need them for ILA, however.
</commit_message>
<xml_diff>
--- a/BrockMirman/BM Table.xlsx
+++ b/BrockMirman/BM Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13880" yWindow="600" windowWidth="10180" windowHeight="15000"/>
+    <workbookView xWindow="14060" yWindow="600" windowWidth="10000" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -154,6 +154,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +473,10 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
@@ -512,7 +513,10 @@
         <f>GSSA!B3</f>
         <v>2.90809E-2</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2">
+        <f>VFI!B3</f>
+        <v>2.7767199999999999E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -530,7 +534,10 @@
         <f>GSSA!C3</f>
         <v>0.40088000000000001</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <f>VFI!C3</f>
+        <v>0.39172000000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
@@ -557,7 +564,10 @@
         <f>GSSA!D3</f>
         <v>6.8293099999999995E-2</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <f>VFI!D3</f>
+        <v>5.9743600000000001E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
@@ -575,7 +585,10 @@
         <f>GSSA!E3</f>
         <v>0.50732500000000003</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <f>VFI!E3</f>
+        <v>0.50685500000000006</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
@@ -595,6 +608,9 @@
       <c r="D9" s="5">
         <v>2.41043E-4</v>
       </c>
+      <c r="E9" s="5">
+        <v>1.0462799999999999E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
@@ -613,22 +629,28 @@
       <c r="C11" s="3">
         <v>1.8518824345174754E-3</v>
       </c>
-      <c r="D11">
-        <v>173.34756409923267</v>
+      <c r="D11" s="3">
+        <v>0.2924845068967401</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.83543701622406852</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="6">
         <v>31.537829729678734</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="6">
         <v>62.380262520635483</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>122.76904415020975</v>
+      </c>
+      <c r="E12" s="6">
+        <v>41.496690635862635</v>
       </c>
     </row>
   </sheetData>
@@ -645,7 +667,7 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
@@ -818,7 +840,7 @@
       <selection activeCell="C3" sqref="C3:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="2:6">
       <c r="C1" t="s">
@@ -992,7 +1014,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
@@ -1162,10 +1184,10 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
@@ -1193,40 +1215,136 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
+      <c r="B3" s="2">
+        <v>2.7767199999999999E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.39172000000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5.9743600000000001E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.50685500000000006</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="2">
+        <v>9.4391700000000002E-3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.13103600000000001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7.2520199999999996E-3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9.08927E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>14</v>
       </c>
+      <c r="B5" s="2">
+        <v>1.52861E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.212204</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.17442E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.47195E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
+      <c r="B6" s="2">
+        <v>2.3426600000000001E-4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.5228999999999999E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.9468200000000002E-3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4.9467199999999999E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>16</v>
       </c>
+      <c r="B7" s="2">
+        <v>0.18878300000000001</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.6207199999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.14504</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.181785</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>17</v>
       </c>
+      <c r="B8" s="2">
+        <v>1.54199E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.212559</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.40787E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.7648400000000002E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>18</v>
       </c>
+      <c r="B9" s="2">
+        <v>2.79055E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.39269399999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>9.0490099999999997E-3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.1825199999999999E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>19</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4.5213700000000002E-3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6.4852300000000002E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>8.7553900000000005E-4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.12542E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added VFI results for ILA to paper.  Cleaned up and deleted old and duplicated files.
</commit_message>
<xml_diff>
--- a/BrockMirman/BM Table.xlsx
+++ b/BrockMirman/BM Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="600" windowWidth="10000" windowHeight="15000"/>
+    <workbookView xWindow="2980" yWindow="600" windowWidth="21080" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="GSSA" sheetId="5" r:id="rId4"/>
     <sheet name="VFI" sheetId="7" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="LIN">Table!$C$3:$C$13</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="22">
   <si>
     <t>EX</t>
   </si>
@@ -91,6 +94,9 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>Tota</t>
   </si>
 </sst>
 </file>
@@ -470,15 +476,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -491,13 +500,25 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -517,8 +538,24 @@
         <f>VFI!B3</f>
         <v>2.7767199999999999E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3" s="3">
+        <f>B3/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f>C3/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <f>D3/LIN</f>
+        <v>1.0041331160311038</v>
+      </c>
+      <c r="J3" s="3">
+        <f>E3/LIN</f>
+        <v>0.95877242655691064</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -538,8 +575,24 @@
         <f>VFI!C3</f>
         <v>0.39172000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G4" s="3">
+        <f>B4/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f>C4/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <f>D4/LIN</f>
+        <v>1.0020647212626295</v>
+      </c>
+      <c r="J4" s="3">
+        <f>E4/LIN</f>
+        <v>0.97916781234533334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -547,8 +600,11 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -568,8 +624,24 @@
         <f>VFI!D3</f>
         <v>5.9743600000000001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="G6" s="3">
+        <f>B6/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f>C6/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <f>D6/LIN</f>
+        <v>0.99987555196364353</v>
+      </c>
+      <c r="J6" s="3">
+        <f>E6/LIN</f>
+        <v>0.87470278880729002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -589,13 +661,32 @@
         <f>VFI!E3</f>
         <v>0.50685500000000006</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G7" s="3">
+        <f>B7/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f>C7/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <f>D7/LIN</f>
+        <v>0.99999802888083789</v>
+      </c>
+      <c r="J7" s="3">
+        <f>E7/LIN</f>
+        <v>0.99907160287468022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1">
+      <c r="G8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" s="5" customFormat="1">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -611,15 +702,34 @@
       <c r="E9" s="5">
         <v>1.0462799999999999E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9" s="3">
+        <f>B9/LIN</f>
+        <v>0.96273333836096542</v>
+      </c>
+      <c r="H9">
+        <f>C9/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <f>D9/LIN</f>
+        <v>0.95674384081987451</v>
+      </c>
+      <c r="J9" s="3">
+        <f>E9/LIN</f>
+        <v>4.1528770624868523</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -635,8 +745,24 @@
       <c r="E11" s="3">
         <v>0.83543701622406852</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="G11" s="4" t="str">
+        <f>B11</f>
+        <v>n/a</v>
+      </c>
+      <c r="H11">
+        <f>C11/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="6">
+        <f>D11/LIN</f>
+        <v>157.9390254181819</v>
+      </c>
+      <c r="J11" s="6">
+        <f>E11/LIN</f>
+        <v>451.12853853584346</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -651,6 +777,59 @@
       </c>
       <c r="E12" s="6">
         <v>41.496690635862635</v>
+      </c>
+      <c r="G12" s="3">
+        <f>B12/LIN</f>
+        <v>0.50557385389723186</v>
+      </c>
+      <c r="H12">
+        <f>C12/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <f>D12/LIN</f>
+        <v>1.968075144114656</v>
+      </c>
+      <c r="J12" s="3">
+        <f>E12/LIN</f>
+        <v>0.66522148126798064</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6">
+        <f>B12</f>
+        <v>31.537829729678734</v>
+      </c>
+      <c r="C13" s="6">
+        <f>C12+C11</f>
+        <v>62.382114403069998</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" ref="D13:E13" si="0">D12+D11</f>
+        <v>123.06152865710649</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>42.332127652086704</v>
+      </c>
+      <c r="G13" s="3">
+        <f>B13/LIN</f>
+        <v>0.50555884537518447</v>
+      </c>
+      <c r="H13">
+        <f>C13/LIN</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <f>D13/LIN</f>
+        <v>1.9727053152121161</v>
+      </c>
+      <c r="J13" s="3">
+        <f>E13/LIN</f>
+        <v>0.67859398574671304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>